<commit_message>
color coded foreign keys
</commit_message>
<xml_diff>
--- a/BCNF Tables.xlsx
+++ b/BCNF Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\University\CS 461\databaseproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hpque_5t\Documents\DatabaseSystems\projectFiles\databaseproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D811FBED-7DD2-4F86-AC3A-91D6B74A7AA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B605B7-DC29-4B18-8E35-1BE03842325C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="9300" windowWidth="20520" windowHeight="18270" xr2:uid="{1B1111D2-451E-46DF-A103-8F16306DA3B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B1111D2-451E-46DF-A103-8F16306DA3B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +291,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,8 +310,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,21 +334,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,34 +661,34 @@
   <dimension ref="B1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
@@ -687,7 +697,7 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
@@ -699,7 +709,7 @@
       <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L2" t="s">
@@ -714,417 +724,417 @@
       <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="1">
         <v>81706</v>
       </c>
-      <c r="I3" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K3" s="9">
+      <c r="I3" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K3" s="4">
         <v>0</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O3" s="6">
+      <c r="N3" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O3" s="1">
         <v>28</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="12">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="1">
         <v>3214</v>
       </c>
-      <c r="I4" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="I4" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K4" s="4">
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O4" s="6">
+      <c r="N4" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O4" s="1">
         <v>41</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="12">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="1">
         <v>83765</v>
       </c>
-      <c r="I5" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K5" s="9">
+      <c r="I5" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K5" s="4">
         <v>2</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="N5" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O5" s="1">
         <v>15</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="12">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="1">
         <v>78846</v>
       </c>
-      <c r="I6" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="I6" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K6" s="4">
         <v>3</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="N6" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O6" s="1">
         <v>47</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="12">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="1">
         <v>80456</v>
       </c>
-      <c r="I7" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K7" s="9">
+      <c r="I7" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K7" s="4">
         <v>4</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O7" s="6">
+      <c r="N7" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O7" s="1">
         <v>46</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="12">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="1">
         <v>2438</v>
       </c>
-      <c r="I8" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="I8" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K8" s="4">
         <v>5</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O8" s="6">
+      <c r="N8" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O8" s="1">
         <v>56</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="12">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="4">
         <v>6</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="1">
         <v>90447</v>
       </c>
-      <c r="I9" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K9" s="9">
+      <c r="I9" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K9" s="4">
         <v>6</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O9" s="6">
+      <c r="N9" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O9" s="1">
         <v>6</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="12">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="4">
         <v>7</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="1">
         <v>25656</v>
       </c>
-      <c r="I10" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K10" s="9">
+      <c r="I10" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K10" s="4">
         <v>7</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N10" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O10" s="6">
+      <c r="N10" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O10" s="1">
         <v>52</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="12">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="4">
         <v>8</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="1">
         <v>7379</v>
       </c>
-      <c r="I11" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K11" s="9">
+      <c r="I11" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K11" s="4">
         <v>8</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O11" s="6">
+      <c r="N11" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O11" s="1">
         <v>41</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="12">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
+      <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="4">
         <v>9</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="1">
         <v>6044</v>
       </c>
-      <c r="I12" s="7">
-        <v>25568</v>
-      </c>
-      <c r="K12" s="9">
+      <c r="I12" s="2">
+        <v>25568</v>
+      </c>
+      <c r="K12" s="4">
         <v>9</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="7">
-        <v>25568</v>
-      </c>
-      <c r="O12" s="6">
+      <c r="N12" s="2">
+        <v>25568</v>
+      </c>
+      <c r="O12" s="1">
         <v>1</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="12">
         <v>43</v>
       </c>
     </row>
@@ -1132,81 +1142,81 @@
       <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="P13" s="6" t="s">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="F20" s="10" t="s">
+      <c r="C20" s="8"/>
+      <c r="F20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="L20" s="5" t="s">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="L20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="M21" t="s">
@@ -1220,214 +1230,214 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
+      <c r="B22" s="12">
         <v>3</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="12">
         <v>26</v>
       </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" s="9">
+      <c r="F22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L22" s="4">
         <v>0</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="1">
         <v>2</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="1">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
+      <c r="B23" s="12">
         <v>5</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="12">
         <v>41</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="4">
         <v>1</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="1">
         <v>4</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="1">
         <v>245</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
+      <c r="B24" s="12">
         <v>7</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="12">
         <v>15</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="4">
         <v>2</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N24" s="6">
+      <c r="N24" s="1">
         <v>1</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25" s="12">
         <v>11</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="12">
         <v>11</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="4">
         <v>3</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="1">
         <v>1</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="1">
         <v>161</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+      <c r="B26" s="12">
         <v>12</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="12">
         <v>20</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="4">
         <v>4</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="M26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="1">
         <v>2</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="1">
         <v>224</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="B27" s="12">
         <v>19</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="12">
         <v>22</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="4">
         <v>5</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="M27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="1">
         <v>4</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+      <c r="B28" s="12">
         <v>20</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="12">
         <v>37</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="4">
         <v>6</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28" s="1">
         <v>1</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="1">
         <v>153</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="B29" s="12">
         <v>28</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="12">
         <v>36</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="4">
         <v>7</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="M29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="1">
         <v>2</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="1">
         <v>169</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+      <c r="B30" s="12">
         <v>36</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="12">
         <v>9</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="4">
         <v>8</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="M30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="1">
         <v>2</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="1">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
+      <c r="B31" s="12">
         <v>47</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="12">
         <v>20</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="4">
         <v>9</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="M31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="1">
         <v>2</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="1">
         <v>24</v>
       </c>
     </row>

</xml_diff>